<commit_message>
Finalised Data Cleansing Part and Modified Minutes Meeting
</commit_message>
<xml_diff>
--- a/assign03_meeting_diary.xlsx
+++ b/assign03_meeting_diary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\SEM 2\ETC5521\assignment-3-amica\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evang\Documents\Monash University\Semester 2\ETC5521\Assignment\Assignment 3\assignment-3-amica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{636A9A44-CD42-482B-9769-73C8F9612195}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6847594B-7373-4A37-A731-13A3E8D8F360}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{AA36F377-8185-6045-958F-09DEEBD07722}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{AA36F377-8185-6045-958F-09DEEBD07722}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
   <si>
     <t>Team Name:</t>
   </si>
@@ -96,6 +96,11 @@
 - Data cleansing to be for Q3 part 2
 - Deadline for Q3 part 2 is 29/09/2023
 - Next meeting on 29/09/2023</t>
+  </si>
+  <si>
+    <t>- Data cleansing finalised
+- Allocate whose going to take which expectation
+- Deadline for Q4 is 02/10/2023</t>
   </si>
 </sst>
 </file>
@@ -146,27 +151,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -481,20 +484,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B0CB73-A0EE-1845-ADEE-622320F90FF1}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="28.69921875" customWidth="1"/>
-    <col min="4" max="4" width="15.69921875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.296875" customWidth="1"/>
+    <col min="1" max="1" width="18.9140625" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -502,7 +505,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -510,20 +513,20 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -540,89 +543,106 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="4">
+    <row r="7" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+      <c r="A7" s="5">
         <v>45186</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="6">
         <v>0.5625</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="6">
         <v>0.60416666666666663</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="93.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="4">
+    <row r="8" spans="1:5" ht="93" x14ac:dyDescent="0.35">
+      <c r="A8" s="5">
         <v>45188</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="6">
         <v>0.91666666666666663</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="6">
         <v>0.9375</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="78" x14ac:dyDescent="0.3">
-      <c r="A9" s="8">
+    <row r="9" spans="1:5" ht="77.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="5">
         <v>45193</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9" s="6">
         <v>0.79166666666666663</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="6">
         <v>0.875</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="78" x14ac:dyDescent="0.3">
-      <c r="A10" s="8">
+    <row r="10" spans="1:5" ht="77.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="5">
         <v>45194</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10" s="6">
         <v>0.83333333333333337</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="6">
         <v>0.875</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A11" s="8">
+    <row r="11" spans="1:5" ht="62" x14ac:dyDescent="0.35">
+      <c r="A11" s="5">
         <v>45196</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B11" s="6">
         <v>0.89583333333333337</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="6">
         <v>0.94444444444444453</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="4" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="62" x14ac:dyDescent="0.35">
+      <c r="A12" s="5">
+        <v>45199</v>
+      </c>
+      <c r="B12" s="6">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C12" s="6">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed q4 harsh and meeting diary updated
</commit_message>
<xml_diff>
--- a/assign03_meeting_diary.xlsx
+++ b/assign03_meeting_diary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evang\Documents\Monash University\Semester 2\ETC5521\Assignment\Assignment 3\assignment-3-amica\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\SEM 2\ETC5521\assignment-3-amica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6847594B-7373-4A37-A731-13A3E8D8F360}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48D6AD9A-D960-497E-979A-DA3B672B7711}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{AA36F377-8185-6045-958F-09DEEBD07722}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{AA36F377-8185-6045-958F-09DEEBD07722}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
   <si>
     <t>Team Name:</t>
   </si>
@@ -101,6 +101,13 @@
     <t>- Data cleansing finalised
 - Allocate whose going to take which expectation
 - Deadline for Q4 is 02/10/2023</t>
+  </si>
+  <si>
+    <t>- Done with Q4
+- Merging of Q4 to be done on 04/10/2023
+- Q5 coding part done by Evan
+- Deadline for Q5 explanation is 05/10/2023
+- Deadline for Q5 VIA is 06/10/2023</t>
   </si>
 </sst>
 </file>
@@ -484,20 +491,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B0CB73-A0EE-1845-ADEE-622320F90FF1}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.9140625" customWidth="1"/>
-    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.33203125" customWidth="1"/>
+    <col min="1" max="1" width="18.8984375" customWidth="1"/>
+    <col min="4" max="4" width="15.69921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -505,7 +512,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -513,20 +520,20 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -543,7 +550,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>45186</v>
       </c>
@@ -560,7 +567,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="93" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>45188</v>
       </c>
@@ -577,7 +584,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="78" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>45193</v>
       </c>
@@ -594,7 +601,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" ht="78" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>45194</v>
       </c>
@@ -611,7 +618,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="62" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>45196</v>
       </c>
@@ -628,7 +635,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="62" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>45199</v>
       </c>
@@ -643,6 +650,23 @@
       </c>
       <c r="E12" s="4" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="78" x14ac:dyDescent="0.3">
+      <c r="A13" s="5">
+        <v>45203</v>
+      </c>
+      <c r="B13" s="6">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="C13" s="6">
+        <v>0.99305555555555547</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated meeting diary and completed AI script file
</commit_message>
<xml_diff>
--- a/assign03_meeting_diary.xlsx
+++ b/assign03_meeting_diary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\SEM 2\ETC5521\assignment-3-amica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48D6AD9A-D960-497E-979A-DA3B672B7711}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEBE5DCA-AF18-43FF-9C35-F70AB5D5AB21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{AA36F377-8185-6045-958F-09DEEBD07722}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
   <si>
     <t>Team Name:</t>
   </si>
@@ -106,6 +106,12 @@
     <t>- Done with Q4
 - Merging of Q4 to be done on 04/10/2023
 - Q5 coding part done by Evan
+- Deadline for Q5 explanation is 05/10/2023
+- Deadline for Q5 VIA is 06/10/2023</t>
+  </si>
+  <si>
+    <t>- Done with Q5 IDA, partial EDA
+- Merged Q5 IDA and reformat the report
 - Deadline for Q5 explanation is 05/10/2023
 - Deadline for Q5 VIA is 06/10/2023</t>
   </si>
@@ -491,7 +497,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B0CB73-A0EE-1845-ADEE-622320F90FF1}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
@@ -669,6 +675,23 @@
         <v>18</v>
       </c>
     </row>
+    <row r="14" spans="1:5" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A14" s="5">
+        <v>45204</v>
+      </c>
+      <c r="B14" s="6">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="C14" s="6">
+        <v>0.99305555555555547</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update meeting diary on Oct 19
</commit_message>
<xml_diff>
--- a/assign03_meeting_diary.xlsx
+++ b/assign03_meeting_diary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\markm\OneDrive\Documents\Monash\ETC5521\Assignment3_2\assignment-3-amica\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chloewang/Desktop/2023-S2/ETC5521 - Exploratory data analysis/Assignment3-2/assignment-3-amica/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{607A6F4C-BD4B-4A46-BAAD-BA53CEE83FD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E61FF0C-9938-AC46-9F67-DC9916DFFECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AA36F377-8185-6045-958F-09DEEBD07722}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="12460" xr2:uid="{AA36F377-8185-6045-958F-09DEEBD07722}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
   <si>
     <t>Team Name:</t>
   </si>
@@ -55,9 +55,6 @@
   </si>
   <si>
     <t>Members present</t>
-  </si>
-  <si>
-    <t>All</t>
   </si>
   <si>
     <t>Discussions</t>
@@ -128,6 +125,16 @@
     <t>- Added necessary files in repo
 - Assinged Tasks to all members
 - Checked for access &amp; cloned repo to local machines</t>
+  </si>
+  <si>
+    <t>Evan Hadinata Ginting (33477558) / Harsh Jain (33397058)</t>
+  </si>
+  <si>
+    <t>Aishwarya Anil Kumar (32644329) / Chih Hui Wang (33209006) / Shreyansh Mahtolia (33509115)</t>
+  </si>
+  <si>
+    <t>- Data description on the tourism dataset is completed.
+- Discussing and analyzing the pattern of tourism</t>
   </si>
 </sst>
 </file>
@@ -178,16 +185,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -197,11 +201,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -517,232 +536,289 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B0CB73-A0EE-1845-ADEE-622320F90FF1}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.8984375" customWidth="1"/>
-    <col min="4" max="4" width="15.69921875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.296875" customWidth="1"/>
+    <col min="1" max="1" width="18.83203125" customWidth="1"/>
+    <col min="2" max="3" width="10.6640625" style="11"/>
+    <col min="4" max="4" width="31.33203125" customWidth="1"/>
+    <col min="5" max="5" width="60.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B1" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
+      <c r="B2" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B3" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B4" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B5" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B6" s="11" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="12" t="s">
         <v>5</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A10" s="4">
         <v>45186</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="5">
         <v>0.5625</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="5">
         <v>0.60416666666666663</v>
       </c>
-      <c r="D10" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="93.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="5">
+      <c r="D10" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="A11" s="4">
         <v>45188</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="5">
         <v>0.91666666666666663</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="5">
         <v>0.9375</v>
       </c>
-      <c r="D11" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="4" t="s">
+      <c r="D11" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A12" s="4">
+        <v>45193</v>
+      </c>
+      <c r="B12" s="5">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="C12" s="5">
+        <v>0.875</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="78" x14ac:dyDescent="0.3">
-      <c r="A12" s="5">
-        <v>45193</v>
-      </c>
-      <c r="B12" s="6">
-        <v>0.79166666666666663</v>
-      </c>
-      <c r="C12" s="6">
+    <row r="13" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="A13" s="4">
+        <v>45194</v>
+      </c>
+      <c r="B13" s="5">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="C13" s="5">
         <v>0.875</v>
       </c>
-      <c r="D12" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="4" t="s">
+      <c r="D13" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="78" x14ac:dyDescent="0.3">
-      <c r="A13" s="5">
-        <v>45194</v>
-      </c>
-      <c r="B13" s="6">
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="C13" s="6">
+    <row r="14" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="A14" s="4">
+        <v>45196</v>
+      </c>
+      <c r="B14" s="5">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="C14" s="5">
+        <v>0.94444444444444453</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A15" s="4">
+        <v>45199</v>
+      </c>
+      <c r="B15" s="5">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C15" s="5">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+      <c r="A16" s="4">
+        <v>45203</v>
+      </c>
+      <c r="B16" s="5">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="C16" s="5">
+        <v>0.99305555555555547</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="A17" s="4">
+        <v>45204</v>
+      </c>
+      <c r="B17" s="5">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="C17" s="5">
+        <v>0.99305555555555547</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A18" s="4">
+        <v>45214</v>
+      </c>
+      <c r="B18" s="5">
         <v>0.875</v>
       </c>
-      <c r="D13" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A14" s="5">
-        <v>45196</v>
-      </c>
-      <c r="B14" s="6">
-        <v>0.89583333333333337</v>
-      </c>
-      <c r="C14" s="6">
-        <v>0.94444444444444453</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A15" s="5">
-        <v>45199</v>
-      </c>
-      <c r="B15" s="6">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="C15" s="6">
-        <v>0.45833333333333331</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="78" x14ac:dyDescent="0.3">
-      <c r="A16" s="5">
-        <v>45203</v>
-      </c>
-      <c r="B16" s="6">
-        <v>0.91666666666666663</v>
-      </c>
-      <c r="C16" s="6">
-        <v>0.99305555555555547</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A17" s="5">
-        <v>45204</v>
-      </c>
-      <c r="B17" s="6">
-        <v>0.95833333333333337</v>
-      </c>
-      <c r="C17" s="6">
-        <v>0.99305555555555547</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A18" s="9">
-        <v>45214</v>
-      </c>
-      <c r="B18" s="8">
-        <v>0.875</v>
-      </c>
-      <c r="C18" s="8">
+      <c r="C18" s="5">
         <v>0.9375</v>
       </c>
-      <c r="D18" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>23</v>
-      </c>
+      <c r="D18" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A19" s="4">
+        <v>45218</v>
+      </c>
+      <c r="B19" s="5">
+        <v>0.625</v>
+      </c>
+      <c r="C19" s="5">
+        <v>0.6875</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="8"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="7"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="8"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="7"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="8"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="7"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="8"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="7"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="8"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="7"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D25" s="7"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D26" s="7"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D27" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update the diary on Oct 22 meeting
</commit_message>
<xml_diff>
--- a/assign03_meeting_diary.xlsx
+++ b/assign03_meeting_diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chloewang/Desktop/2023-S2/ETC5521 - Exploratory data analysis/Assignment3-2/assignment-3-amica/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E61FF0C-9938-AC46-9F67-DC9916DFFECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D2783B6-F53D-4744-B43A-74BA45A9C8FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="12460" xr2:uid="{AA36F377-8185-6045-958F-09DEEBD07722}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
   <si>
     <t>Team Name:</t>
   </si>
@@ -135,6 +135,11 @@
   <si>
     <t>- Data description on the tourism dataset is completed.
 - Discussing and analyzing the pattern of tourism</t>
+  </si>
+  <si>
+    <t>- Discuss and fix the error issues with the Chuck 19 left join
+- Discuss the next steps for the analysis section, next meeting, the date of completion and the date of recording
+- Discussion of the completed section: IDA and temporal analysis (keep or delete plots)</t>
   </si>
 </sst>
 </file>
@@ -185,7 +190,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -218,9 +223,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -538,8 +540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B0CB73-A0EE-1845-ADEE-622320F90FF1}">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -777,20 +779,30 @@
       <c r="D19" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="E19" s="13" t="s">
+      <c r="E19" s="10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="8"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="7"/>
+    <row r="20" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+      <c r="A20" s="4">
+        <v>45221</v>
+      </c>
+      <c r="B20" s="5">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="C20" s="5">
+        <v>0.99305555555555547</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="8"/>
       <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
       <c r="D21" s="7"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -813,6 +825,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D25" s="7"/>
+      <c r="E25" s="10"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D26" s="7"/>

</xml_diff>

<commit_message>
update meeting diary on Oct 25 evening
</commit_message>
<xml_diff>
--- a/assign03_meeting_diary.xlsx
+++ b/assign03_meeting_diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chloewang/Desktop/2023-S2/ETC5521 - Exploratory data analysis/Assignment3-2/assignment-3-amica/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D2783B6-F53D-4744-B43A-74BA45A9C8FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F65C2443-E3D6-9B4C-94F5-E4F9325C94AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="12460" xr2:uid="{AA36F377-8185-6045-958F-09DEEBD07722}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
   <si>
     <t>Team Name:</t>
   </si>
@@ -133,13 +133,18 @@
     <t>Aishwarya Anil Kumar (32644329) / Chih Hui Wang (33209006) / Shreyansh Mahtolia (33509115)</t>
   </si>
   <si>
-    <t>- Data description on the tourism dataset is completed.
-- Discussing and analyzing the pattern of tourism</t>
-  </si>
-  <si>
     <t>- Discuss and fix the error issues with the Chuck 19 left join
 - Discuss the next steps for the analysis section, next meeting, the date of completion and the date of recording
 - Discussion of the completed section: IDA and temporal analysis (keep or delete plots)</t>
+  </si>
+  <si>
+    <t>- Data description on the tourism dataset is completed.
+- Discussing and analyzing the pattern of tourism.</t>
+  </si>
+  <si>
+    <t>- Discussion on the analysis and plot to be retained in the tourism section.
+- Assigning each individual section of the report for the presentation.
+- Determining the practice time for the next presentation.</t>
   </si>
 </sst>
 </file>
@@ -190,7 +195,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -210,9 +215,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
@@ -223,6 +225,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -541,22 +555,22 @@
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.83203125" customWidth="1"/>
-    <col min="2" max="3" width="10.6640625" style="11"/>
+    <col min="2" max="3" width="10.6640625" style="10"/>
     <col min="4" max="4" width="31.33203125" customWidth="1"/>
-    <col min="5" max="5" width="60.33203125" customWidth="1"/>
+    <col min="5" max="5" width="105.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>8</v>
       </c>
     </row>
@@ -564,27 +578,27 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="10" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="10" t="s">
         <v>21</v>
       </c>
     </row>
@@ -600,10 +614,10 @@
       <c r="A9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="11" t="s">
         <v>5</v>
       </c>
       <c r="D9" s="2" t="s">
@@ -623,10 +637,10 @@
       <c r="C10" s="5">
         <v>0.60416666666666663</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="9" t="s">
         <v>10</v>
       </c>
     </row>
@@ -640,10 +654,10 @@
       <c r="C11" s="5">
         <v>0.9375</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="9" t="s">
         <v>12</v>
       </c>
     </row>
@@ -657,10 +671,10 @@
       <c r="C12" s="5">
         <v>0.875</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E12" s="9" t="s">
         <v>13</v>
       </c>
     </row>
@@ -674,10 +688,10 @@
       <c r="C13" s="5">
         <v>0.875</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="9" t="s">
         <v>14</v>
       </c>
     </row>
@@ -691,10 +705,10 @@
       <c r="C14" s="5">
         <v>0.94444444444444453</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E14" s="9" t="s">
         <v>15</v>
       </c>
     </row>
@@ -708,10 +722,10 @@
       <c r="C15" s="5">
         <v>0.45833333333333331</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="E15" s="9" t="s">
         <v>16</v>
       </c>
     </row>
@@ -725,10 +739,10 @@
       <c r="C16" s="5">
         <v>0.99305555555555547</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E16" s="9" t="s">
         <v>17</v>
       </c>
     </row>
@@ -742,10 +756,10 @@
       <c r="C17" s="5">
         <v>0.99305555555555547</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D17" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E17" s="9" t="s">
         <v>18</v>
       </c>
     </row>
@@ -759,10 +773,10 @@
       <c r="C18" s="5">
         <v>0.9375</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D18" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="E18" s="9" t="s">
         <v>22</v>
       </c>
     </row>
@@ -776,14 +790,14 @@
       <c r="C19" s="5">
         <v>0.6875</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="D19" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="E19" s="10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+      <c r="E19" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
         <v>45221</v>
       </c>
@@ -793,39 +807,51 @@
       <c r="C20" s="5">
         <v>0.99305555555555547</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="D20" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="E20" s="10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="8"/>
-      <c r="B21" s="6"/>
-      <c r="D21" s="7"/>
+      <c r="E20" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A21" s="4">
+        <v>45224</v>
+      </c>
+      <c r="B21" s="5">
+        <v>0.8125</v>
+      </c>
+      <c r="C21" s="14">
+        <v>0.84027777777777779</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="8"/>
+      <c r="A22" s="6"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
       <c r="D22" s="7"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="8"/>
+      <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
       <c r="D23" s="7"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="8"/>
+      <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
       <c r="D24" s="7"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D25" s="7"/>
-      <c r="E25" s="10"/>
+      <c r="E25" s="9"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D26" s="7"/>

</xml_diff>

<commit_message>
Update dairy for Oct 26 morning meeting
</commit_message>
<xml_diff>
--- a/assign03_meeting_diary.xlsx
+++ b/assign03_meeting_diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chloewang/Desktop/2023-S2/ETC5521 - Exploratory data analysis/Assignment3-2/assignment-3-amica/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F65C2443-E3D6-9B4C-94F5-E4F9325C94AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{844F627A-C8AC-6E4A-B5B8-F25C0E0211E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="12460" xr2:uid="{AA36F377-8185-6045-958F-09DEEBD07722}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
   <si>
     <t>Team Name:</t>
   </si>
@@ -145,6 +145,12 @@
     <t>- Discussion on the analysis and plot to be retained in the tourism section.
 - Assigning each individual section of the report for the presentation.
 - Determining the practice time for the next presentation.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Discuss the final draft report and decide the way to present (create a new branch to presentation)
+- Discuss the allocation of remaining tasks
+- Prepare and decide content for recording the video. 
+- Decide the next meeting time for practice and go through report for presentation </t>
   </si>
 </sst>
 </file>
@@ -195,7 +201,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -231,12 +237,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -555,7 +555,7 @@
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -821,25 +821,36 @@
       <c r="B21" s="5">
         <v>0.8125</v>
       </c>
-      <c r="C21" s="14">
+      <c r="C21" s="5">
         <v>0.84027777777777779</v>
       </c>
       <c r="D21" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="E21" s="15" t="s">
+      <c r="E21" s="9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="6"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="7"/>
+    <row r="22" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="A22" s="4">
+        <v>45225</v>
+      </c>
+      <c r="B22" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="C22" s="5">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="6"/>
-      <c r="B23" s="6"/>
+      <c r="A23" s="4"/>
+      <c r="B23" s="5"/>
       <c r="C23" s="6"/>
       <c r="D23" s="7"/>
     </row>

</xml_diff>

<commit_message>
update diary on Oct 26 evening meeting
</commit_message>
<xml_diff>
--- a/assign03_meeting_diary.xlsx
+++ b/assign03_meeting_diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chloewang/Desktop/2023-S2/ETC5521 - Exploratory data analysis/Assignment3-2/assignment-3-amica/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{844F627A-C8AC-6E4A-B5B8-F25C0E0211E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B743D8C-9B52-8144-B551-DD588750E85E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="12460" xr2:uid="{AA36F377-8185-6045-958F-09DEEBD07722}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
   <si>
     <t>Team Name:</t>
   </si>
@@ -151,6 +151,10 @@
 - Discuss the allocation of remaining tasks
 - Prepare and decide content for recording the video. 
 - Decide the next meeting time for practice and go through report for presentation </t>
+  </si>
+  <si>
+    <t>- Practice presentation
+- Discuss presentation final report.</t>
   </si>
 </sst>
 </file>
@@ -554,8 +558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B0CB73-A0EE-1845-ADEE-622320F90FF1}">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -848,11 +852,22 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="4"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="7"/>
+    <row r="23" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A23" s="4">
+        <v>45225</v>
+      </c>
+      <c r="B23" s="5">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="C23" s="5">
+        <v>0.8125</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="6"/>

</xml_diff>

<commit_message>
update diary for meeing on Oct 26 night
</commit_message>
<xml_diff>
--- a/assign03_meeting_diary.xlsx
+++ b/assign03_meeting_diary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chloewang/Desktop/2023-S2/ETC5521 - Exploratory data analysis/Assignment3-2/assignment-3-amica/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B743D8C-9B52-8144-B551-DD588750E85E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{920A3F19-63CC-0346-BBB9-88D522A517DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="12460" xr2:uid="{AA36F377-8185-6045-958F-09DEEBD07722}"/>
+    <workbookView xWindow="1060" yWindow="560" windowWidth="28800" windowHeight="12460" xr2:uid="{AA36F377-8185-6045-958F-09DEEBD07722}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
   <si>
     <t>Team Name:</t>
   </si>
@@ -155,6 +155,10 @@
   <si>
     <t>- Practice presentation
 - Discuss presentation final report.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Practice presentation part within our team and other team
+- Record the presentation with other teams </t>
   </si>
 </sst>
 </file>
@@ -205,7 +209,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -216,9 +220,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -558,14 +559,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B0CB73-A0EE-1845-ADEE-622320F90FF1}">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.83203125" customWidth="1"/>
-    <col min="2" max="3" width="10.6640625" style="10"/>
+    <col min="2" max="3" width="10.6640625" style="9"/>
     <col min="4" max="4" width="31.33203125" customWidth="1"/>
     <col min="5" max="5" width="105.5" customWidth="1"/>
   </cols>
@@ -574,7 +575,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>8</v>
       </c>
     </row>
@@ -582,27 +583,27 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>21</v>
       </c>
     </row>
@@ -618,10 +619,10 @@
       <c r="A9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="10" t="s">
         <v>5</v>
       </c>
       <c r="D9" s="2" t="s">
@@ -641,10 +642,10 @@
       <c r="C10" s="5">
         <v>0.60416666666666663</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="8" t="s">
         <v>10</v>
       </c>
     </row>
@@ -658,10 +659,10 @@
       <c r="C11" s="5">
         <v>0.9375</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="8" t="s">
         <v>12</v>
       </c>
     </row>
@@ -675,10 +676,10 @@
       <c r="C12" s="5">
         <v>0.875</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E12" s="8" t="s">
         <v>13</v>
       </c>
     </row>
@@ -692,10 +693,10 @@
       <c r="C13" s="5">
         <v>0.875</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="8" t="s">
         <v>14</v>
       </c>
     </row>
@@ -709,10 +710,10 @@
       <c r="C14" s="5">
         <v>0.94444444444444453</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E14" s="8" t="s">
         <v>15</v>
       </c>
     </row>
@@ -726,10 +727,10 @@
       <c r="C15" s="5">
         <v>0.45833333333333331</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="E15" s="8" t="s">
         <v>16</v>
       </c>
     </row>
@@ -743,10 +744,10 @@
       <c r="C16" s="5">
         <v>0.99305555555555547</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="E16" s="8" t="s">
         <v>17</v>
       </c>
     </row>
@@ -760,10 +761,10 @@
       <c r="C17" s="5">
         <v>0.99305555555555547</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="E17" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -777,10 +778,10 @@
       <c r="C18" s="5">
         <v>0.9375</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="E18" s="8" t="s">
         <v>22</v>
       </c>
     </row>
@@ -794,10 +795,10 @@
       <c r="C19" s="5">
         <v>0.6875</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D19" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E19" s="12" t="s">
+      <c r="E19" s="11" t="s">
         <v>26</v>
       </c>
     </row>
@@ -811,10 +812,10 @@
       <c r="C20" s="5">
         <v>0.99305555555555547</v>
       </c>
-      <c r="D20" s="13" t="s">
+      <c r="D20" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="E20" s="9" t="s">
+      <c r="E20" s="8" t="s">
         <v>25</v>
       </c>
     </row>
@@ -828,10 +829,10 @@
       <c r="C21" s="5">
         <v>0.84027777777777779</v>
       </c>
-      <c r="D21" s="13" t="s">
+      <c r="D21" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="E21" s="9" t="s">
+      <c r="E21" s="8" t="s">
         <v>27</v>
       </c>
     </row>
@@ -845,10 +846,10 @@
       <c r="C22" s="5">
         <v>0.54166666666666663</v>
       </c>
-      <c r="D22" s="13" t="s">
+      <c r="D22" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="E22" s="9" t="s">
+      <c r="E22" s="8" t="s">
         <v>28</v>
       </c>
     </row>
@@ -862,28 +863,39 @@
       <c r="C23" s="5">
         <v>0.8125</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="D23" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="E23" s="9" t="s">
+      <c r="E23" s="8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="6"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="7"/>
+    <row r="24" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A24" s="4">
+        <v>45225</v>
+      </c>
+      <c r="B24" s="5">
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="C24" s="5">
+        <v>0.93055555555555547</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D25" s="7"/>
-      <c r="E25" s="9"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="8"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D26" s="7"/>
+      <c r="D26" s="6"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D27" s="7"/>
+      <c r="D27" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update a new discussion on Oct 27
</commit_message>
<xml_diff>
--- a/assign03_meeting_diary.xlsx
+++ b/assign03_meeting_diary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chloewang/Desktop/2023-S2/ETC5521 - Exploratory data analysis/Assignment3-2/assignment-3-amica/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{920A3F19-63CC-0346-BBB9-88D522A517DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32D4A731-814A-0D44-86B5-1EF985553094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="560" windowWidth="28800" windowHeight="12460" xr2:uid="{AA36F377-8185-6045-958F-09DEEBD07722}"/>
+    <workbookView xWindow="0" yWindow="560" windowWidth="28800" windowHeight="12460" xr2:uid="{AA36F377-8185-6045-958F-09DEEBD07722}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="32">
   <si>
     <t>Team Name:</t>
   </si>
@@ -159,6 +159,11 @@
   <si>
     <t xml:space="preserve">- Practice presentation part within our team and other team
 - Record the presentation with other teams </t>
+  </si>
+  <si>
+    <t>- Discuss and modify the final report version.
+- Make minor corrections.
+- Discuss video presentation submission.</t>
   </si>
 </sst>
 </file>
@@ -560,7 +565,7 @@
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -887,9 +892,22 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D25" s="6"/>
-      <c r="E25" s="8"/>
+    <row r="25" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A25" s="4">
+        <v>45226</v>
+      </c>
+      <c r="B25" s="5">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="C25" s="5">
+        <v>0.625</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D26" s="6"/>

</xml_diff>